<commit_message>
fixed some errors in the result files
</commit_message>
<xml_diff>
--- a/results/2024_01_21_round1.xlsx
+++ b/results/2024_01_21_round1.xlsx
@@ -41,7 +41,7 @@
     <t>12:00</t>
   </si>
   <si>
-    <t>12:40</t>
+    <t>12:25</t>
   </si>
   <si>
     <t>Table 1</t>
@@ -53,7 +53,7 @@
     <t>Group A</t>
   </si>
   <si>
-    <t>Bertalan Pusztai</t>
+    <t>Berci Pusztai</t>
   </si>
   <si>
     <t>1</t>
@@ -74,34 +74,46 @@
     <t>Ákos Szvetnik</t>
   </si>
   <si>
-    <t>12:45</t>
+    <t>12:30</t>
+  </si>
+  <si>
+    <t>12:55</t>
+  </si>
+  <si>
+    <t>Dani Pusztai</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Máté Vass</t>
+  </si>
+  <si>
+    <t>Dáni Gyulai-Nagy</t>
+  </si>
+  <si>
+    <t>Laci Ferenczi</t>
+  </si>
+  <si>
+    <t>13:00</t>
   </si>
   <si>
     <t>13:25</t>
   </si>
   <si>
-    <t>Dani Pusztai</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Máté Vass</t>
-  </si>
-  <si>
-    <t>Dáni Gyulai-Nagy</t>
-  </si>
-  <si>
-    <t>Laci Ferenczi</t>
-  </si>
-  <si>
     <t>13:30</t>
   </si>
   <si>
-    <t>14:10</t>
-  </si>
-  <si>
-    <t>14:15</t>
+    <t>13:55</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>14:25</t>
+  </si>
+  <si>
+    <t>14:30</t>
   </si>
   <si>
     <t>14:55</t>
@@ -110,10 +122,16 @@
     <t>15:00</t>
   </si>
   <si>
-    <t>15:40</t>
-  </si>
-  <si>
-    <t>15:45</t>
+    <t>15:25</t>
+  </si>
+  <si>
+    <t>15:30</t>
+  </si>
+  <si>
+    <t>15:55</t>
+  </si>
+  <si>
+    <t>16:00</t>
   </si>
   <si>
     <t>16:25</t>
@@ -122,10 +140,16 @@
     <t>16:30</t>
   </si>
   <si>
-    <t>17:10</t>
-  </si>
-  <si>
-    <t>17:15</t>
+    <t>16:55</t>
+  </si>
+  <si>
+    <t>17:00</t>
+  </si>
+  <si>
+    <t>17:25</t>
+  </si>
+  <si>
+    <t>17:30</t>
   </si>
   <si>
     <t>17:55</t>
@@ -134,64 +158,40 @@
     <t>18:00</t>
   </si>
   <si>
-    <t>18:40</t>
-  </si>
-  <si>
-    <t>18:45</t>
+    <t>18:25</t>
+  </si>
+  <si>
+    <t>18:30</t>
+  </si>
+  <si>
+    <t>18:55</t>
+  </si>
+  <si>
+    <t>19:00</t>
   </si>
   <si>
     <t>19:25</t>
   </si>
   <si>
+    <t>Knockout phase</t>
+  </si>
+  <si>
+    <t>Match B1</t>
+  </si>
+  <si>
+    <t>3*</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Match B2</t>
+  </si>
+  <si>
     <t>19:30</t>
   </si>
   <si>
-    <t>20:10</t>
-  </si>
-  <si>
-    <t>20:15</t>
-  </si>
-  <si>
-    <t>20:55</t>
-  </si>
-  <si>
-    <t>21:00</t>
-  </si>
-  <si>
-    <t>21:40</t>
-  </si>
-  <si>
-    <t>21:45</t>
-  </si>
-  <si>
-    <t>22:25</t>
-  </si>
-  <si>
-    <t>22:30</t>
-  </si>
-  <si>
-    <t>23:10</t>
-  </si>
-  <si>
-    <t>Knockout phase</t>
-  </si>
-  <si>
-    <t>Match B1</t>
-  </si>
-  <si>
-    <t>3*</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Match B2</t>
-  </si>
-  <si>
-    <t>23:15</t>
-  </si>
-  <si>
-    <t>23:55</t>
+    <t>19:55</t>
   </si>
   <si>
     <t>Match B3</t>

</xml_diff>

<commit_message>
added results outside from Tournify
</commit_message>
<xml_diff>
--- a/results/2024_01_21_round1.xlsx
+++ b/results/2024_01_21_round1.xlsx
@@ -1,10 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matevass/Documents/Programming/R/darts-statistics/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61C108D-8094-DF4C-BC5C-DA773988E521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -206,13 +217,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-    </font>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -220,24 +226,13 @@
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none">
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -246,19 +241,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="1" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -583,969 +584,982 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="2" t="s">
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="2" t="s">
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
+      <c r="I15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="2" t="s">
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="2" t="s">
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="2" t="s">
+      <c r="G18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="2" t="s">
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="2" t="s">
+      <c r="G19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="2" t="s">
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="2" t="s">
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="2" t="s">
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="2" t="s">
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="2" t="s">
+      <c r="G22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
         <v>26</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="2" t="s">
+      <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I23" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="2" t="s">
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="2" t="s">
+      <c r="G24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="2" t="s">
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" t="s">
         <v>24</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" t="s">
         <v>20</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="s">
+      <c r="I25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="2" t="s">
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="2" t="s">
+      <c r="G26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="s">
         <v>19</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="2" t="s">
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" s="2" t="s">
+      <c r="G27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I27" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="2" t="s">
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" t="s">
         <v>26</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="2" t="s">
+      <c r="G28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" t="s">
         <v>20</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="2" t="s">
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
         <v>27</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="s">
+      <c r="I29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" t="s">
         <v>55</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" t="s">
         <v>14</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" t="s">
         <v>56</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" t="s">
         <v>25</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" t="s">
         <v>58</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" t="s">
         <v>26</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" t="s">
         <v>61</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" t="s">
         <v>14</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" t="s">
         <v>57</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" t="s">
         <v>26</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I32" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
         <v>59</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" t="s">
         <v>60</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" t="s">
         <v>63</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" t="s">
         <v>25</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" t="s">
         <v>24</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" t="s">
         <v>27</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="I33" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>